<commit_message>
Waiting for post fix
</commit_message>
<xml_diff>
--- a/app/Recursos Marcas/Blunua/Plantilla modificada.xlsx
+++ b/app/Recursos Marcas/Blunua/Plantilla modificada.xlsx
@@ -373,7 +373,7 @@
     <t>Gris</t>
   </si>
   <si>
-    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Corazón+Definido/Collar+Corazขn+Definido+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Corazón+Definido/Collar+Corazขn+Definido+2+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Corazón+Definido/Collar+Corazขn+Definido+3+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Corazón+Definido/Collar+Corazขn+Definido+4+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Corazón+Definido/Collar+Corazขn+Definido+5+Amarillo.jpg']</t>
+    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Coraz%E0%B8%82n+Definido/Collar+Corazขn+Definido+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Coraz%E0%B8%82n+Definido/Collar+Corazขn+Definido+2+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Coraz%E0%B8%82n+Definido/Collar+Corazขn+Definido+3+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Coraz%E0%B8%82n+Definido/Collar+Corazขn+Definido+4+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Collar+Coraz%E0%B8%82n+Definido/Collar+Corazขn+Definido+5+Amarillo.jpg']</t>
   </si>
   <si>
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Delicadeza/Candongas+Delicadeza+1+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Delicadeza/Candongas+Delicadeza+2+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Delicadeza/Candongas+Delicadeza+3+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Delicadeza/Candongas+Delicadeza+4+Rosa.jpg']</t>
@@ -385,7 +385,7 @@
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Anillo+ZigZag/Anillo+ZigZag+1+Gris.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Anillo+ZigZag/Anillo+ZigZag+2+Rosa.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Anillo+ZigZag/Anillo+ZigZag+3+Amarillo.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Anillo+ZigZag/Anillo+ZigZag+4+Negro.jpg']</t>
   </si>
   <si>
-    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Básicos+Mini/Topitos+B\xa0sicos+Mini+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Básicos+Mini/Topitos+B\xa0sicos+Mini+2+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Básicos+Mini/Topitos+B\xa0sicos+Mini+3+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Básicos+Mini/Topitos+B\xa0sicos+Mini+4+Gris.jpg']</t>
+    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+B%C2%A0sicos+Mini/Topitos+B\xa0sicos+Mini+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+B%C2%A0sicos+Mini/Topitos+B\xa0sicos+Mini+2+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+B%C2%A0sicos+Mini/Topitos+B\xa0sicos+Mini+3+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+B%C2%A0sicos+Mini/Topitos+B\xa0sicos+Mini+4+Gris.jpg']</t>
   </si>
   <si>
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Lucero+Mini/Topitos+Lucero+Mini+1+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Lucero+Mini/Topitos+Lucero+Mini+2+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Topitos+Lucero+Mini/Topitos+Lucero+Mini+3+Amarillo.jpg']</t>
@@ -397,10 +397,10 @@
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+1+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+2+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+3+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+4+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+5+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Earcuff+ZigZag/Earcuff+ZigZag+6+Negro.jpg']</t>
   </si>
   <si>
-    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+2+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+3+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+4+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+5+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Corazón/Candongas+Corazขn+6+Negro.jpg']</t>
-  </si>
-  <si>
-    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelación+Mini/Candongas+Constelaciขn+Mini+1+Gris.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelación+Mini/Candongas+Constelaciขn+Mini+2+Rosa.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelación+Mini/Candongas+Constelaciขn+Mini+3+Amarillo.png']</t>
+    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+1+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+2+Amarillo.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+3+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+4+Gris.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+5+Negro.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Coraz%E0%B8%82n/Candongas+Corazขn+6+Negro.jpg']</t>
+  </si>
+  <si>
+    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelaci%E0%B8%82n+Mini/Candongas+Constelaciขn+Mini+1+Gris.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelaci%E0%B8%82n+Mini/Candongas+Constelaciขn+Mini+2+Rosa.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Candongas+Constelaci%E0%B8%82n+Mini/Candongas+Constelaciขn+Mini+3+Amarillo.png']</t>
   </si>
   <si>
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Choker+Clarity/Choker+Clarity+1+Rosa.jpg', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Choker+Clarity/Choker+Clarity+2+Amarillo.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Blunua/Choker+Clarity/Choker+Clarity+3+Gris.png']</t>

</xml_diff>